<commit_message>
fixing bugs on financial survey
</commit_message>
<xml_diff>
--- a/hybris-sagia/hybris/bin/custom/sagia/sagiabackoffice/resources/backoffice/file/financeSurvey.xlsx
+++ b/hybris-sagia/hybris/bin/custom/sagia/sagiabackoffice/resources/backoffice/file/financeSurvey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohmbad/projects/personal/financeSurvey/misacommerce/hybris-sagia/hybris/bin/custom/sagia/sagiabackoffice/resources/backoffice/file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B94A6-6EDC-4B4A-B7BF-F52AEED8157F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED7D13D-32D4-3A4E-B816-AE5F0183BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35260" yWindow="-2300" windowWidth="34120" windowHeight="17500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33180" yWindow="-4380" windowWidth="48740" windowHeight="18600" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="company profile" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t xml:space="preserve">Customer ID </t>
   </si>
@@ -135,6 +135,129 @@
   </si>
   <si>
     <t>Total Shareholder Equity (Current Quarter)</t>
+  </si>
+  <si>
+    <t>Shareholder Type</t>
+  </si>
+  <si>
+    <t>(Entity) Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Current Nationality</t>
+  </si>
+  <si>
+    <t>Residence Country / Entity Country</t>
+  </si>
+  <si>
+    <t>Shares Percentage</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Voting Power</t>
+  </si>
+  <si>
+    <t>Preferred shares in the company</t>
+  </si>
+  <si>
+    <t>Value Of Reverse Investment</t>
+  </si>
+  <si>
+    <t>Trade Debit (current quarter)</t>
+  </si>
+  <si>
+    <t>Short and Long term loans  (current quarter)</t>
+  </si>
+  <si>
+    <t>Interest received on loans and receivables  (current quarter)</t>
+  </si>
+  <si>
+    <t>Dividends received Dividends received  (current quarter)</t>
+  </si>
+  <si>
+    <t>Expenses received  (current quarter)</t>
+  </si>
+  <si>
+    <t>Sell of production supplies  (current quarter)</t>
+  </si>
+  <si>
+    <t>Sell of machinery and equipment  (current quarter)</t>
+  </si>
+  <si>
+    <t>Current debit account  (current quarter)</t>
+  </si>
+  <si>
+    <t>Expenses received (current quarter)</t>
+  </si>
+  <si>
+    <t>Insurance commission receivable  (current quarter)</t>
+  </si>
+  <si>
+    <t>Trade Credit (current quarter)</t>
+  </si>
+  <si>
+    <t>Short and Long term loans - paid (current quarter)</t>
+  </si>
+  <si>
+    <t>Interest payable on loans and payables (current quarter)</t>
+  </si>
+  <si>
+    <t>Dividends paid (current quarter)</t>
+  </si>
+  <si>
+    <t>Expenses paid (current quarter)</t>
+  </si>
+  <si>
+    <t>Purchase of production supplies (current quarter)</t>
+  </si>
+  <si>
+    <t>Purchase of machinery and equipment (current quarter)</t>
+  </si>
+  <si>
+    <t>Current credit account (current quarter)</t>
+  </si>
+  <si>
+    <t>Insurance commission payable  (current quarter)</t>
+  </si>
+  <si>
+    <t>Other - please specify (current quarter)</t>
+  </si>
+  <si>
+    <t>Total liabilities (current quarter)</t>
+  </si>
+  <si>
+    <t>Equity -  Additional Paid Up Capital (current quarter)</t>
+  </si>
+  <si>
+    <t>Retained Earnings (current quarter)</t>
+  </si>
+  <si>
+    <t>Profit (Loss) (Current Quarter )</t>
+  </si>
+  <si>
+    <t>Other Debit (current quarter)</t>
+  </si>
+  <si>
+    <t>Total  Debit (current quarter)</t>
+  </si>
+  <si>
+    <t>Shareholder Equity Others (current quarter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affiliate Type </t>
+  </si>
+  <si>
+    <t>Entity Sector</t>
+  </si>
+  <si>
+    <t>Entity Subsector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Entity a Mutlinational Company </t>
   </si>
 </sst>
 </file>
@@ -546,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FA1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -872,7 +995,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -973,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA74B6C7-1F7F-6444-AD3F-107AF79E9796}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1042,24 +1165,361 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4164E9-38CC-B747-A35C-1BE12164F958}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="L1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:AK1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="31.5" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+    <col min="11" max="11" width="46.33203125" customWidth="1"/>
+    <col min="12" max="12" width="53" customWidth="1"/>
+    <col min="13" max="13" width="60.83203125" customWidth="1"/>
+    <col min="14" max="14" width="46.6640625" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" customWidth="1"/>
+    <col min="16" max="16" width="51" customWidth="1"/>
+    <col min="17" max="17" width="45.83203125" customWidth="1"/>
+    <col min="18" max="18" width="40.6640625" customWidth="1"/>
+    <col min="19" max="19" width="47.1640625" customWidth="1"/>
+    <col min="20" max="20" width="43.1640625" customWidth="1"/>
+    <col min="21" max="21" width="38.1640625" customWidth="1"/>
+    <col min="22" max="22" width="32.33203125" customWidth="1"/>
+    <col min="23" max="23" width="48.33203125" customWidth="1"/>
+    <col min="24" max="24" width="38.33203125" customWidth="1"/>
+    <col min="25" max="25" width="28.83203125" customWidth="1"/>
+    <col min="26" max="26" width="31.33203125" customWidth="1"/>
+    <col min="27" max="27" width="44" customWidth="1"/>
+    <col min="28" max="28" width="90.83203125" customWidth="1"/>
+    <col min="29" max="29" width="43.5" customWidth="1"/>
+    <col min="30" max="30" width="30.6640625" customWidth="1"/>
+    <col min="31" max="31" width="54.5" customWidth="1"/>
+    <col min="32" max="32" width="63" customWidth="1"/>
+    <col min="33" max="33" width="30.33203125" customWidth="1"/>
+    <col min="34" max="34" width="52.33203125" customWidth="1"/>
+    <col min="35" max="35" width="42.83203125" customWidth="1"/>
+    <col min="36" max="36" width="37.1640625" customWidth="1"/>
+    <col min="37" max="37" width="34.33203125" customWidth="1"/>
+    <col min="38" max="38" width="42.83203125" customWidth="1"/>
+    <col min="39" max="39" width="47.83203125" customWidth="1"/>
+    <col min="40" max="40" width="39.33203125" customWidth="1"/>
+    <col min="41" max="41" width="44" customWidth="1"/>
+    <col min="42" max="42" width="30.5" customWidth="1"/>
+    <col min="43" max="43" width="45.1640625" customWidth="1"/>
+    <col min="44" max="44" width="28.83203125" customWidth="1"/>
+    <col min="45" max="45" width="32.83203125" customWidth="1"/>
+    <col min="46" max="46" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA6BB70-2F03-7F48-925E-BA992F231999}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="11" max="11" width="42.1640625" customWidth="1"/>
+    <col min="12" max="12" width="42.83203125" customWidth="1"/>
+    <col min="13" max="13" width="42.5" customWidth="1"/>
+    <col min="14" max="14" width="36.1640625" customWidth="1"/>
+    <col min="15" max="15" width="59.6640625" customWidth="1"/>
+    <col min="16" max="16" width="51.83203125" customWidth="1"/>
+    <col min="17" max="17" width="49.83203125" customWidth="1"/>
+    <col min="18" max="18" width="56" customWidth="1"/>
+    <col min="19" max="19" width="32.33203125" customWidth="1"/>
+    <col min="20" max="20" width="47.5" customWidth="1"/>
+    <col min="21" max="21" width="47.1640625" customWidth="1"/>
+    <col min="22" max="22" width="60.6640625" customWidth="1"/>
+    <col min="23" max="23" width="32" customWidth="1"/>
+    <col min="24" max="24" width="48.1640625" customWidth="1"/>
+    <col min="25" max="25" width="44.1640625" customWidth="1"/>
+    <col min="26" max="26" width="45" customWidth="1"/>
+    <col min="27" max="27" width="42" customWidth="1"/>
+    <col min="28" max="28" width="35" customWidth="1"/>
+    <col min="29" max="29" width="37.83203125" customWidth="1"/>
+    <col min="30" max="30" width="51.1640625" customWidth="1"/>
+    <col min="31" max="31" width="48.6640625" customWidth="1"/>
+    <col min="32" max="32" width="45.5" customWidth="1"/>
+    <col min="33" max="33" width="52.33203125" customWidth="1"/>
+    <col min="34" max="34" width="36.6640625" customWidth="1"/>
+    <col min="35" max="35" width="49.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>